<commit_message>
Modify: Slightly fixed the cell range typo of "Program Area" in Pattern III.
</commit_message>
<xml_diff>
--- a/docs/Format comparison and example.xlsx
+++ b/docs/Format comparison and example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{4CB0F0A3-3E6A-4B77-84EE-CC1515F3F2B8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{739C4746-120C-4494-AD21-294C34CEC37C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2025,10 +2025,103 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="84" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2036,42 +2129,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="84" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2081,52 +2138,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="80" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="82" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2162,10 +2177,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="80" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="83" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2186,6 +2204,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2196,25 +2215,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="83" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2542,51 +2542,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:43" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
       <c r="I1" s="84"/>
     </row>
     <row r="2" spans="2:43" x14ac:dyDescent="0.2">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="G2" s="104" t="s">
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="G2" s="123" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="104"/>
+      <c r="H2" s="123"/>
     </row>
     <row r="3" spans="2:43" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:43" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="107"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="113"/>
     </row>
     <row r="5" spans="2:43" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="93" t="s">
+      <c r="D5" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="94"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="93"/>
       <c r="H5" s="9" t="s">
         <v>12</v>
       </c>
@@ -2596,14 +2596,14 @@
         <v>3</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="94"/>
-      <c r="F6" s="93" t="s">
+      <c r="E6" s="93"/>
+      <c r="F6" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="94"/>
+      <c r="G6" s="93"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="2:43" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -2611,11 +2611,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="94" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="96"/>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="94" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="96"/>
@@ -2702,72 +2702,72 @@
       <c r="E12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="91" t="s">
+      <c r="F12" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="92"/>
+      <c r="G12" s="87"/>
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="2:43" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:43" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="106"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="107"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="113"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="105" t="s">
+      <c r="K14" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="106"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="106"/>
-      <c r="O14" s="106"/>
-      <c r="P14" s="106"/>
-      <c r="Q14" s="106"/>
-      <c r="R14" s="106"/>
-      <c r="S14" s="106"/>
-      <c r="T14" s="106"/>
-      <c r="U14" s="106"/>
-      <c r="V14" s="106"/>
-      <c r="W14" s="106"/>
-      <c r="X14" s="107"/>
+      <c r="L14" s="112"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="112"/>
+      <c r="O14" s="112"/>
+      <c r="P14" s="112"/>
+      <c r="Q14" s="112"/>
+      <c r="R14" s="112"/>
+      <c r="S14" s="112"/>
+      <c r="T14" s="112"/>
+      <c r="U14" s="112"/>
+      <c r="V14" s="112"/>
+      <c r="W14" s="112"/>
+      <c r="X14" s="113"/>
       <c r="Z14" s="5"/>
-      <c r="AA14" s="105" t="s">
+      <c r="AA14" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="AB14" s="106"/>
-      <c r="AC14" s="106"/>
-      <c r="AD14" s="106"/>
-      <c r="AE14" s="106"/>
-      <c r="AF14" s="106"/>
-      <c r="AG14" s="106"/>
-      <c r="AH14" s="106"/>
-      <c r="AI14" s="106"/>
-      <c r="AJ14" s="106"/>
-      <c r="AK14" s="106"/>
-      <c r="AL14" s="106"/>
-      <c r="AM14" s="106"/>
-      <c r="AN14" s="106"/>
-      <c r="AO14" s="106"/>
-      <c r="AP14" s="106"/>
-      <c r="AQ14" s="107"/>
+      <c r="AB14" s="112"/>
+      <c r="AC14" s="112"/>
+      <c r="AD14" s="112"/>
+      <c r="AE14" s="112"/>
+      <c r="AF14" s="112"/>
+      <c r="AG14" s="112"/>
+      <c r="AH14" s="112"/>
+      <c r="AI14" s="112"/>
+      <c r="AJ14" s="112"/>
+      <c r="AK14" s="112"/>
+      <c r="AL14" s="112"/>
+      <c r="AM14" s="112"/>
+      <c r="AN14" s="112"/>
+      <c r="AO14" s="112"/>
+      <c r="AP14" s="112"/>
+      <c r="AQ14" s="113"/>
     </row>
     <row r="15" spans="2:43" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="93" t="s">
+      <c r="D15" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="108"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="94"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="93"/>
       <c r="H15" s="9" t="s">
         <v>12</v>
       </c>
@@ -2775,20 +2775,20 @@
       <c r="K15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="93" t="s">
+      <c r="L15" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="M15" s="108"/>
-      <c r="N15" s="108"/>
-      <c r="O15" s="108"/>
-      <c r="P15" s="108"/>
-      <c r="Q15" s="108"/>
-      <c r="R15" s="108"/>
-      <c r="S15" s="108"/>
-      <c r="T15" s="108"/>
-      <c r="U15" s="108"/>
-      <c r="V15" s="108"/>
-      <c r="W15" s="94"/>
+      <c r="M15" s="92"/>
+      <c r="N15" s="92"/>
+      <c r="O15" s="92"/>
+      <c r="P15" s="92"/>
+      <c r="Q15" s="92"/>
+      <c r="R15" s="92"/>
+      <c r="S15" s="92"/>
+      <c r="T15" s="92"/>
+      <c r="U15" s="92"/>
+      <c r="V15" s="92"/>
+      <c r="W15" s="93"/>
       <c r="X15" s="9" t="s">
         <v>12</v>
       </c>
@@ -2796,23 +2796,23 @@
       <c r="AA15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AB15" s="93" t="s">
+      <c r="AB15" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="AC15" s="108"/>
-      <c r="AD15" s="108"/>
-      <c r="AE15" s="108"/>
-      <c r="AF15" s="108"/>
-      <c r="AG15" s="108"/>
-      <c r="AH15" s="108"/>
-      <c r="AI15" s="108"/>
-      <c r="AJ15" s="108"/>
-      <c r="AK15" s="108"/>
-      <c r="AL15" s="108"/>
-      <c r="AM15" s="94"/>
-      <c r="AN15" s="32"/>
-      <c r="AO15" s="32"/>
-      <c r="AP15" s="32"/>
+      <c r="AC15" s="92"/>
+      <c r="AD15" s="92"/>
+      <c r="AE15" s="92"/>
+      <c r="AF15" s="92"/>
+      <c r="AG15" s="92"/>
+      <c r="AH15" s="92"/>
+      <c r="AI15" s="92"/>
+      <c r="AJ15" s="92"/>
+      <c r="AK15" s="92"/>
+      <c r="AL15" s="92"/>
+      <c r="AM15" s="92"/>
+      <c r="AN15" s="92"/>
+      <c r="AO15" s="92"/>
+      <c r="AP15" s="93"/>
       <c r="AQ15" s="9" t="s">
         <v>12</v>
       </c>
@@ -2822,75 +2822,75 @@
         <v>3</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="93" t="s">
+      <c r="D16" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="108"/>
-      <c r="F16" s="108"/>
-      <c r="G16" s="94"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="93"/>
       <c r="H16" s="2"/>
       <c r="J16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K16" s="1"/>
-      <c r="L16" s="93" t="s">
+      <c r="L16" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="94"/>
-      <c r="N16" s="93" t="s">
+      <c r="M16" s="93"/>
+      <c r="N16" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="94"/>
-      <c r="P16" s="93" t="s">
+      <c r="O16" s="93"/>
+      <c r="P16" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="94"/>
-      <c r="R16" s="93" t="s">
+      <c r="Q16" s="93"/>
+      <c r="R16" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="S16" s="94"/>
-      <c r="T16" s="93" t="s">
+      <c r="S16" s="93"/>
+      <c r="T16" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="U16" s="94"/>
-      <c r="V16" s="93" t="s">
+      <c r="U16" s="93"/>
+      <c r="V16" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="W16" s="94"/>
+      <c r="W16" s="93"/>
       <c r="X16" s="2"/>
       <c r="Z16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="AA16" s="1"/>
-      <c r="AB16" s="93" t="s">
+      <c r="AB16" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="AC16" s="94"/>
-      <c r="AD16" s="93" t="s">
+      <c r="AC16" s="93"/>
+      <c r="AD16" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AE16" s="94"/>
-      <c r="AF16" s="93" t="s">
+      <c r="AE16" s="93"/>
+      <c r="AF16" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AG16" s="94"/>
-      <c r="AH16" s="93" t="s">
+      <c r="AG16" s="93"/>
+      <c r="AH16" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="AI16" s="94"/>
-      <c r="AJ16" s="93" t="s">
+      <c r="AI16" s="93"/>
+      <c r="AJ16" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="AK16" s="94"/>
-      <c r="AL16" s="93" t="s">
+      <c r="AK16" s="93"/>
+      <c r="AL16" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AM16" s="94"/>
-      <c r="AN16" s="93" t="s">
+      <c r="AM16" s="93"/>
+      <c r="AN16" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="AO16" s="108"/>
-      <c r="AP16" s="94"/>
+      <c r="AO16" s="92"/>
+      <c r="AP16" s="93"/>
       <c r="AQ16" s="2"/>
     </row>
     <row r="17" spans="2:43" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -2898,38 +2898,38 @@
         <v>2</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="95" t="s">
+      <c r="D17" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
       <c r="G17" s="96"/>
       <c r="H17" s="2"/>
       <c r="J17" s="6" t="s">
         <v>2</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="95" t="s">
+      <c r="L17" s="94" t="s">
         <v>24</v>
       </c>
       <c r="M17" s="96"/>
-      <c r="N17" s="95" t="s">
+      <c r="N17" s="94" t="s">
         <v>32</v>
       </c>
       <c r="O17" s="96"/>
-      <c r="P17" s="95" t="s">
+      <c r="P17" s="94" t="s">
         <v>33</v>
       </c>
       <c r="Q17" s="96"/>
-      <c r="R17" s="95" t="s">
+      <c r="R17" s="94" t="s">
         <v>35</v>
       </c>
       <c r="S17" s="96"/>
-      <c r="T17" s="95" t="s">
+      <c r="T17" s="94" t="s">
         <v>35</v>
       </c>
       <c r="U17" s="96"/>
-      <c r="V17" s="95" t="s">
+      <c r="V17" s="94" t="s">
         <v>38</v>
       </c>
       <c r="W17" s="96"/>
@@ -2938,34 +2938,34 @@
         <v>2</v>
       </c>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="95" t="s">
+      <c r="AB17" s="94" t="s">
         <v>24</v>
       </c>
       <c r="AC17" s="96"/>
-      <c r="AD17" s="95" t="s">
+      <c r="AD17" s="94" t="s">
         <v>32</v>
       </c>
       <c r="AE17" s="96"/>
-      <c r="AF17" s="95" t="s">
+      <c r="AF17" s="94" t="s">
         <v>33</v>
       </c>
       <c r="AG17" s="96"/>
-      <c r="AH17" s="95" t="s">
+      <c r="AH17" s="94" t="s">
         <v>35</v>
       </c>
       <c r="AI17" s="96"/>
-      <c r="AJ17" s="95" t="s">
+      <c r="AJ17" s="94" t="s">
         <v>35</v>
       </c>
       <c r="AK17" s="96"/>
-      <c r="AL17" s="95" t="s">
+      <c r="AL17" s="94" t="s">
         <v>47</v>
       </c>
       <c r="AM17" s="96"/>
-      <c r="AN17" s="95" t="s">
+      <c r="AN17" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="AO17" s="98"/>
+      <c r="AO17" s="95"/>
       <c r="AP17" s="96"/>
       <c r="AQ17" s="2"/>
     </row>
@@ -2977,11 +2977,11 @@
       <c r="D18" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="109" t="s">
+      <c r="E18" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="110"/>
-      <c r="G18" s="111"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="99"/>
       <c r="H18" s="2"/>
       <c r="J18" s="6" t="s">
         <v>6</v>
@@ -3064,10 +3064,10 @@
       <c r="AM18" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AN18" s="100" t="s">
+      <c r="AN18" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="AO18" s="101"/>
+      <c r="AO18" s="110"/>
       <c r="AP18" s="20" t="s">
         <v>5</v>
       </c>
@@ -3081,11 +3081,11 @@
       <c r="D19" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="112" t="s">
+      <c r="E19" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="113"/>
-      <c r="G19" s="114"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="102"/>
       <c r="H19" s="2"/>
       <c r="J19" s="6" t="s">
         <v>8</v>
@@ -3187,11 +3187,11 @@
       <c r="D20" s="25">
         <v>150</v>
       </c>
-      <c r="E20" s="115" t="s">
+      <c r="E20" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="116"/>
-      <c r="G20" s="117"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="105"/>
       <c r="H20" s="4"/>
       <c r="J20" s="7" t="s">
         <v>19</v>
@@ -3291,11 +3291,11 @@
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="118" t="s">
+      <c r="E21" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="119"/>
-      <c r="G21" s="86"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="116"/>
       <c r="H21" s="14"/>
       <c r="J21" s="11" t="s">
         <v>15</v>
@@ -3306,24 +3306,24 @@
         <v>28</v>
       </c>
       <c r="N21" s="78"/>
-      <c r="O21" s="97" t="s">
+      <c r="O21" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="P21" s="97"/>
-      <c r="Q21" s="97" t="s">
+      <c r="P21" s="117"/>
+      <c r="Q21" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="R21" s="97"/>
+      <c r="R21" s="117"/>
       <c r="S21" s="38" t="s">
         <v>36</v>
       </c>
       <c r="T21" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="U21" s="85" t="s">
+      <c r="U21" s="88" t="s">
         <v>115</v>
       </c>
-      <c r="V21" s="86"/>
+      <c r="V21" s="116"/>
       <c r="W21" s="79" t="s">
         <v>39</v>
       </c>
@@ -3337,11 +3337,11 @@
         <v>28</v>
       </c>
       <c r="AD21" s="13"/>
-      <c r="AE21" s="85" t="s">
+      <c r="AE21" s="88" t="s">
         <v>31</v>
       </c>
       <c r="AF21" s="90"/>
-      <c r="AG21" s="85" t="s">
+      <c r="AG21" s="88" t="s">
         <v>42</v>
       </c>
       <c r="AH21" s="90"/>
@@ -3351,14 +3351,14 @@
       <c r="AJ21" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="AK21" s="97" t="s">
+      <c r="AK21" s="117" t="s">
         <v>112</v>
       </c>
-      <c r="AL21" s="97"/>
-      <c r="AM21" s="102" t="s">
+      <c r="AL21" s="117"/>
+      <c r="AM21" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="AN21" s="103"/>
+      <c r="AN21" s="122"/>
       <c r="AO21" s="78"/>
       <c r="AP21" s="74" t="s">
         <v>46</v>
@@ -3371,11 +3371,11 @@
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="17"/>
-      <c r="E22" s="91" t="s">
+      <c r="E22" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="99"/>
-      <c r="G22" s="92"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="87"/>
       <c r="H22" s="18"/>
       <c r="J22" s="15" t="s">
         <v>16</v>
@@ -3385,26 +3385,26 @@
       <c r="M22" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="N22" s="91" t="s">
+      <c r="N22" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="92"/>
-      <c r="P22" s="91" t="s">
+      <c r="O22" s="87"/>
+      <c r="P22" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="Q22" s="92"/>
-      <c r="R22" s="91" t="s">
+      <c r="Q22" s="87"/>
+      <c r="R22" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="S22" s="92"/>
-      <c r="T22" s="91" t="s">
+      <c r="S22" s="87"/>
+      <c r="T22" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="U22" s="92"/>
-      <c r="V22" s="91" t="s">
+      <c r="U22" s="87"/>
+      <c r="V22" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="W22" s="92"/>
+      <c r="W22" s="87"/>
       <c r="X22" s="18"/>
       <c r="Z22" s="15" t="s">
         <v>16</v>
@@ -3414,119 +3414,119 @@
       <c r="AC22" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="AD22" s="91" t="s">
+      <c r="AD22" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="AE22" s="92"/>
-      <c r="AF22" s="91" t="s">
+      <c r="AE22" s="87"/>
+      <c r="AF22" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="AG22" s="92"/>
-      <c r="AH22" s="91" t="s">
+      <c r="AG22" s="87"/>
+      <c r="AH22" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="AI22" s="92"/>
-      <c r="AJ22" s="91" t="s">
+      <c r="AI22" s="87"/>
+      <c r="AJ22" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="AK22" s="92"/>
-      <c r="AL22" s="91" t="s">
+      <c r="AK22" s="87"/>
+      <c r="AL22" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="AM22" s="92"/>
-      <c r="AN22" s="91" t="s">
+      <c r="AM22" s="87"/>
+      <c r="AN22" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="AO22" s="99"/>
-      <c r="AP22" s="92"/>
+      <c r="AO22" s="86"/>
+      <c r="AP22" s="87"/>
       <c r="AQ22" s="18"/>
     </row>
     <row r="23" spans="2:43" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="2:43" x14ac:dyDescent="0.2">
-      <c r="Z24" s="89" t="s">
+      <c r="Z24" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="AA24" s="89"/>
-      <c r="AB24" s="89"/>
-      <c r="AC24" s="89"/>
-      <c r="AD24" s="89"/>
-      <c r="AE24" s="89"/>
-      <c r="AF24" s="89"/>
-      <c r="AG24" s="89"/>
-      <c r="AH24" s="89"/>
-      <c r="AI24" s="89"/>
-      <c r="AJ24" s="89"/>
-      <c r="AK24" s="89"/>
-      <c r="AL24" s="89"/>
-      <c r="AM24" s="89"/>
-      <c r="AN24" s="89"/>
-      <c r="AO24" s="89"/>
+      <c r="AA24" s="120"/>
+      <c r="AB24" s="120"/>
+      <c r="AC24" s="120"/>
+      <c r="AD24" s="120"/>
+      <c r="AE24" s="120"/>
+      <c r="AF24" s="120"/>
+      <c r="AG24" s="120"/>
+      <c r="AH24" s="120"/>
+      <c r="AI24" s="120"/>
+      <c r="AJ24" s="120"/>
+      <c r="AK24" s="120"/>
+      <c r="AL24" s="120"/>
+      <c r="AM24" s="120"/>
+      <c r="AN24" s="120"/>
+      <c r="AO24" s="120"/>
     </row>
     <row r="25" spans="2:43" x14ac:dyDescent="0.2">
-      <c r="Z25" s="88" t="s">
+      <c r="Z25" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="AA25" s="88"/>
-      <c r="AB25" s="88"/>
-      <c r="AC25" s="88"/>
-      <c r="AD25" s="88"/>
-      <c r="AE25" s="88"/>
-      <c r="AF25" s="88"/>
-      <c r="AG25" s="88"/>
-      <c r="AH25" s="88"/>
-      <c r="AI25" s="88"/>
-      <c r="AJ25" s="88"/>
-      <c r="AK25" s="88"/>
-      <c r="AL25" s="88"/>
-      <c r="AM25" s="88"/>
-      <c r="AN25" s="88"/>
-      <c r="AO25" s="88"/>
+      <c r="AA25" s="119"/>
+      <c r="AB25" s="119"/>
+      <c r="AC25" s="119"/>
+      <c r="AD25" s="119"/>
+      <c r="AE25" s="119"/>
+      <c r="AF25" s="119"/>
+      <c r="AG25" s="119"/>
+      <c r="AH25" s="119"/>
+      <c r="AI25" s="119"/>
+      <c r="AJ25" s="119"/>
+      <c r="AK25" s="119"/>
+      <c r="AL25" s="119"/>
+      <c r="AM25" s="119"/>
+      <c r="AN25" s="119"/>
+      <c r="AO25" s="119"/>
     </row>
     <row r="28" spans="2:43" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="2:43" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Z29" s="5"/>
-      <c r="AA29" s="105" t="s">
+      <c r="AA29" s="111" t="s">
         <v>120</v>
       </c>
-      <c r="AB29" s="106"/>
-      <c r="AC29" s="106"/>
-      <c r="AD29" s="106"/>
-      <c r="AE29" s="106"/>
-      <c r="AF29" s="106"/>
-      <c r="AG29" s="106"/>
-      <c r="AH29" s="106"/>
-      <c r="AI29" s="106"/>
-      <c r="AJ29" s="106"/>
-      <c r="AK29" s="106"/>
-      <c r="AL29" s="106"/>
-      <c r="AM29" s="106"/>
-      <c r="AN29" s="106"/>
-      <c r="AO29" s="106"/>
-      <c r="AP29" s="106"/>
-      <c r="AQ29" s="107"/>
+      <c r="AB29" s="112"/>
+      <c r="AC29" s="112"/>
+      <c r="AD29" s="112"/>
+      <c r="AE29" s="112"/>
+      <c r="AF29" s="112"/>
+      <c r="AG29" s="112"/>
+      <c r="AH29" s="112"/>
+      <c r="AI29" s="112"/>
+      <c r="AJ29" s="112"/>
+      <c r="AK29" s="112"/>
+      <c r="AL29" s="112"/>
+      <c r="AM29" s="112"/>
+      <c r="AN29" s="112"/>
+      <c r="AO29" s="112"/>
+      <c r="AP29" s="112"/>
+      <c r="AQ29" s="113"/>
     </row>
     <row r="30" spans="2:43" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Z30" s="6"/>
       <c r="AA30" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AB30" s="93" t="s">
+      <c r="AB30" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="AC30" s="108"/>
-      <c r="AD30" s="108"/>
-      <c r="AE30" s="108"/>
-      <c r="AF30" s="108"/>
-      <c r="AG30" s="108"/>
-      <c r="AH30" s="108"/>
-      <c r="AI30" s="108"/>
-      <c r="AJ30" s="108"/>
-      <c r="AK30" s="108"/>
-      <c r="AL30" s="108"/>
-      <c r="AM30" s="94"/>
-      <c r="AN30" s="32"/>
-      <c r="AO30" s="32"/>
-      <c r="AP30" s="32"/>
+      <c r="AC30" s="92"/>
+      <c r="AD30" s="92"/>
+      <c r="AE30" s="92"/>
+      <c r="AF30" s="92"/>
+      <c r="AG30" s="92"/>
+      <c r="AH30" s="92"/>
+      <c r="AI30" s="92"/>
+      <c r="AJ30" s="92"/>
+      <c r="AK30" s="92"/>
+      <c r="AL30" s="92"/>
+      <c r="AM30" s="92"/>
+      <c r="AN30" s="92"/>
+      <c r="AO30" s="92"/>
+      <c r="AP30" s="93"/>
       <c r="AQ30" s="9" t="s">
         <v>12</v>
       </c>
@@ -3536,25 +3536,25 @@
         <v>3</v>
       </c>
       <c r="AA31" s="1"/>
-      <c r="AB31" s="93" t="s">
+      <c r="AB31" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="AC31" s="108"/>
-      <c r="AD31" s="108"/>
-      <c r="AE31" s="108"/>
-      <c r="AF31" s="108"/>
-      <c r="AG31" s="108"/>
-      <c r="AH31" s="108"/>
-      <c r="AI31" s="108"/>
-      <c r="AJ31" s="108"/>
-      <c r="AK31" s="108"/>
-      <c r="AL31" s="108"/>
-      <c r="AM31" s="94"/>
-      <c r="AN31" s="93" t="s">
+      <c r="AC31" s="92"/>
+      <c r="AD31" s="92"/>
+      <c r="AE31" s="92"/>
+      <c r="AF31" s="92"/>
+      <c r="AG31" s="92"/>
+      <c r="AH31" s="92"/>
+      <c r="AI31" s="92"/>
+      <c r="AJ31" s="92"/>
+      <c r="AK31" s="92"/>
+      <c r="AL31" s="92"/>
+      <c r="AM31" s="93"/>
+      <c r="AN31" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="AO31" s="108"/>
-      <c r="AP31" s="94"/>
+      <c r="AO31" s="92"/>
+      <c r="AP31" s="93"/>
       <c r="AQ31" s="2"/>
     </row>
     <row r="32" spans="2:43" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -3562,25 +3562,25 @@
         <v>2</v>
       </c>
       <c r="AA32" s="1"/>
-      <c r="AB32" s="95" t="s">
+      <c r="AB32" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="AC32" s="98"/>
-      <c r="AD32" s="98"/>
-      <c r="AE32" s="98"/>
-      <c r="AF32" s="98"/>
-      <c r="AG32" s="98"/>
-      <c r="AH32" s="98"/>
-      <c r="AI32" s="98"/>
-      <c r="AJ32" s="98"/>
-      <c r="AK32" s="98"/>
-      <c r="AL32" s="98"/>
+      <c r="AC32" s="95"/>
+      <c r="AD32" s="95"/>
+      <c r="AE32" s="95"/>
+      <c r="AF32" s="95"/>
+      <c r="AG32" s="95"/>
+      <c r="AH32" s="95"/>
+      <c r="AI32" s="95"/>
+      <c r="AJ32" s="95"/>
+      <c r="AK32" s="95"/>
+      <c r="AL32" s="95"/>
       <c r="AM32" s="96"/>
-      <c r="AN32" s="148" t="s">
+      <c r="AN32" s="106" t="s">
         <v>119</v>
       </c>
-      <c r="AO32" s="149"/>
-      <c r="AP32" s="150"/>
+      <c r="AO32" s="107"/>
+      <c r="AP32" s="108"/>
       <c r="AQ32" s="2"/>
     </row>
     <row r="33" spans="26:43" x14ac:dyDescent="0.2">
@@ -3591,23 +3591,23 @@
       <c r="AB33" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AC33" s="109" t="s">
+      <c r="AC33" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="AD33" s="110"/>
-      <c r="AE33" s="110"/>
-      <c r="AF33" s="110"/>
-      <c r="AG33" s="110"/>
-      <c r="AH33" s="110"/>
-      <c r="AI33" s="110"/>
-      <c r="AJ33" s="110"/>
-      <c r="AK33" s="110"/>
-      <c r="AL33" s="110"/>
-      <c r="AM33" s="111"/>
-      <c r="AN33" s="100" t="s">
+      <c r="AD33" s="98"/>
+      <c r="AE33" s="98"/>
+      <c r="AF33" s="98"/>
+      <c r="AG33" s="98"/>
+      <c r="AH33" s="98"/>
+      <c r="AI33" s="98"/>
+      <c r="AJ33" s="98"/>
+      <c r="AK33" s="98"/>
+      <c r="AL33" s="98"/>
+      <c r="AM33" s="99"/>
+      <c r="AN33" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="AO33" s="101"/>
+      <c r="AO33" s="110"/>
       <c r="AP33" s="29" t="s">
         <v>5</v>
       </c>
@@ -3621,19 +3621,19 @@
       <c r="AB34" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="AC34" s="112" t="s">
+      <c r="AC34" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="AD34" s="113"/>
-      <c r="AE34" s="113"/>
-      <c r="AF34" s="113"/>
-      <c r="AG34" s="113"/>
-      <c r="AH34" s="113"/>
-      <c r="AI34" s="113"/>
-      <c r="AJ34" s="113"/>
-      <c r="AK34" s="113"/>
-      <c r="AL34" s="113"/>
-      <c r="AM34" s="114"/>
+      <c r="AD34" s="101"/>
+      <c r="AE34" s="101"/>
+      <c r="AF34" s="101"/>
+      <c r="AG34" s="101"/>
+      <c r="AH34" s="101"/>
+      <c r="AI34" s="101"/>
+      <c r="AJ34" s="101"/>
+      <c r="AK34" s="101"/>
+      <c r="AL34" s="101"/>
+      <c r="AM34" s="102"/>
       <c r="AN34" s="26" t="s">
         <v>49</v>
       </c>
@@ -3653,19 +3653,19 @@
       <c r="AB35" s="25">
         <v>150</v>
       </c>
-      <c r="AC35" s="115" t="s">
+      <c r="AC35" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="AD35" s="116"/>
-      <c r="AE35" s="116"/>
-      <c r="AF35" s="116"/>
-      <c r="AG35" s="116"/>
-      <c r="AH35" s="116"/>
-      <c r="AI35" s="116"/>
-      <c r="AJ35" s="116"/>
-      <c r="AK35" s="116"/>
-      <c r="AL35" s="116"/>
-      <c r="AM35" s="117"/>
+      <c r="AD35" s="104"/>
+      <c r="AE35" s="104"/>
+      <c r="AF35" s="104"/>
+      <c r="AG35" s="104"/>
+      <c r="AH35" s="104"/>
+      <c r="AI35" s="104"/>
+      <c r="AJ35" s="104"/>
+      <c r="AK35" s="104"/>
+      <c r="AL35" s="104"/>
+      <c r="AM35" s="105"/>
       <c r="AN35" s="25">
         <v>75</v>
       </c>
@@ -3683,20 +3683,20 @@
       </c>
       <c r="AA36" s="12"/>
       <c r="AB36" s="13"/>
-      <c r="AC36" s="85" t="s">
+      <c r="AC36" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="AD36" s="119"/>
-      <c r="AE36" s="119"/>
-      <c r="AF36" s="119"/>
-      <c r="AG36" s="119"/>
-      <c r="AH36" s="119"/>
-      <c r="AI36" s="119"/>
-      <c r="AJ36" s="119"/>
-      <c r="AK36" s="119"/>
-      <c r="AL36" s="119"/>
-      <c r="AM36" s="119"/>
-      <c r="AN36" s="119"/>
+      <c r="AD36" s="89"/>
+      <c r="AE36" s="89"/>
+      <c r="AF36" s="89"/>
+      <c r="AG36" s="89"/>
+      <c r="AH36" s="89"/>
+      <c r="AI36" s="89"/>
+      <c r="AJ36" s="89"/>
+      <c r="AK36" s="89"/>
+      <c r="AL36" s="89"/>
+      <c r="AM36" s="89"/>
+      <c r="AN36" s="89"/>
       <c r="AO36" s="90"/>
       <c r="AP36" s="77" t="s">
         <v>117</v>
@@ -3709,41 +3709,88 @@
       </c>
       <c r="AA37" s="16"/>
       <c r="AB37" s="17"/>
-      <c r="AC37" s="91" t="s">
+      <c r="AC37" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="AD37" s="99"/>
-      <c r="AE37" s="99"/>
-      <c r="AF37" s="99"/>
-      <c r="AG37" s="99"/>
-      <c r="AH37" s="99"/>
-      <c r="AI37" s="99"/>
-      <c r="AJ37" s="99"/>
-      <c r="AK37" s="99"/>
-      <c r="AL37" s="99"/>
-      <c r="AM37" s="92"/>
-      <c r="AN37" s="91" t="s">
+      <c r="AD37" s="86"/>
+      <c r="AE37" s="86"/>
+      <c r="AF37" s="86"/>
+      <c r="AG37" s="86"/>
+      <c r="AH37" s="86"/>
+      <c r="AI37" s="86"/>
+      <c r="AJ37" s="86"/>
+      <c r="AK37" s="86"/>
+      <c r="AL37" s="86"/>
+      <c r="AM37" s="87"/>
+      <c r="AN37" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="AO37" s="99"/>
-      <c r="AP37" s="92"/>
+      <c r="AO37" s="86"/>
+      <c r="AP37" s="87"/>
       <c r="AQ37" s="18"/>
     </row>
     <row r="38" spans="26:43" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="AN37:AP37"/>
-    <mergeCell ref="AC36:AO36"/>
-    <mergeCell ref="AC37:AM37"/>
-    <mergeCell ref="AB31:AM31"/>
-    <mergeCell ref="AB32:AM32"/>
-    <mergeCell ref="AC33:AM33"/>
-    <mergeCell ref="AC34:AM34"/>
-    <mergeCell ref="AC35:AM35"/>
-    <mergeCell ref="AN32:AP32"/>
-    <mergeCell ref="AN33:AO33"/>
+    <mergeCell ref="AB30:AP30"/>
+    <mergeCell ref="Z25:AO25"/>
+    <mergeCell ref="Z24:AO24"/>
+    <mergeCell ref="AG21:AH21"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AJ16:AK16"/>
+    <mergeCell ref="AJ17:AK17"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AK21:AL21"/>
+    <mergeCell ref="AN17:AP17"/>
+    <mergeCell ref="AN22:AP22"/>
+    <mergeCell ref="AN18:AO18"/>
+    <mergeCell ref="AM21:AN21"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AD17:AE17"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="AB15:AP15"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AD22:AE22"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AL22:AM22"/>
+    <mergeCell ref="AH17:AI17"/>
+    <mergeCell ref="AE21:AF21"/>
+    <mergeCell ref="AA14:AQ14"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AF16:AG16"/>
+    <mergeCell ref="AL16:AM16"/>
+    <mergeCell ref="AN16:AP16"/>
+    <mergeCell ref="AH16:AI16"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="L15:W15"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="K14:X14"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="V17:W17"/>
     <mergeCell ref="AA29:AQ29"/>
-    <mergeCell ref="AB30:AM30"/>
     <mergeCell ref="AN31:AP31"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="C4:H4"/>
@@ -3758,63 +3805,16 @@
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="D16:G16"/>
     <mergeCell ref="D17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="K14:X14"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="L15:W15"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="AA14:AQ14"/>
-    <mergeCell ref="AB15:AM15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AF16:AG16"/>
-    <mergeCell ref="AL16:AM16"/>
-    <mergeCell ref="AN16:AP16"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AD22:AE22"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="AL22:AM22"/>
-    <mergeCell ref="AH17:AI17"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="AE21:AF21"/>
-    <mergeCell ref="AH16:AI16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AD17:AE17"/>
-    <mergeCell ref="AF17:AG17"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="Z25:AO25"/>
-    <mergeCell ref="Z24:AO24"/>
-    <mergeCell ref="AG21:AH21"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ16:AK16"/>
-    <mergeCell ref="AJ17:AK17"/>
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AK21:AL21"/>
-    <mergeCell ref="AN17:AP17"/>
-    <mergeCell ref="AN22:AP22"/>
-    <mergeCell ref="AN18:AO18"/>
-    <mergeCell ref="AM21:AN21"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="AN37:AP37"/>
+    <mergeCell ref="AC36:AO36"/>
+    <mergeCell ref="AC37:AM37"/>
+    <mergeCell ref="AB31:AM31"/>
+    <mergeCell ref="AB32:AM32"/>
+    <mergeCell ref="AC33:AM33"/>
+    <mergeCell ref="AC34:AM34"/>
+    <mergeCell ref="AC35:AM35"/>
+    <mergeCell ref="AN32:AP32"/>
+    <mergeCell ref="AN33:AO33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3843,41 +3843,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
     </row>
     <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:11" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="107"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="113"/>
     </row>
     <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
       <c r="H6" s="32"/>
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
@@ -3890,19 +3890,19 @@
         <v>3</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="93" t="s">
+      <c r="D7" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="94"/>
-      <c r="F7" s="93" t="s">
+      <c r="E7" s="93"/>
+      <c r="F7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="94"/>
-      <c r="H7" s="93" t="s">
+      <c r="G7" s="93"/>
+      <c r="H7" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="108"/>
-      <c r="J7" s="94"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="93"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -3910,18 +3910,18 @@
         <v>2</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="95" t="s">
+      <c r="D8" s="94" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="96"/>
-      <c r="F8" s="95" t="s">
+      <c r="F8" s="94" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="96"/>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="98"/>
+      <c r="I8" s="95"/>
       <c r="J8" s="96"/>
       <c r="K8" s="2"/>
     </row>
@@ -3942,10 +3942,10 @@
       <c r="G9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="100" t="s">
+      <c r="H9" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="101"/>
+      <c r="I9" s="110"/>
       <c r="J9" s="20" t="s">
         <v>5</v>
       </c>
@@ -4080,10 +4080,10 @@
         <v>28</v>
       </c>
       <c r="F14" s="80"/>
-      <c r="G14" s="132" t="s">
+      <c r="G14" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="132"/>
+      <c r="H14" s="125"/>
       <c r="I14" s="80"/>
       <c r="J14" s="68" t="s">
         <v>46</v>
@@ -4101,11 +4101,11 @@
         <v>45000</v>
       </c>
       <c r="F15" s="81"/>
-      <c r="G15" s="122">
+      <c r="G15" s="127">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-2,0)</f>
         <v>139804</v>
       </c>
-      <c r="H15" s="122"/>
+      <c r="H15" s="127"/>
       <c r="I15" s="81"/>
       <c r="J15" s="82">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-2,0)</f>
@@ -4123,10 +4123,10 @@
         <v>94654</v>
       </c>
       <c r="F16" s="83"/>
-      <c r="G16" s="121">
+      <c r="G16" s="126">
         <v>754</v>
       </c>
-      <c r="H16" s="121"/>
+      <c r="H16" s="126"/>
       <c r="I16" s="83"/>
       <c r="J16" s="70">
         <v>408442</v>
@@ -4142,15 +4142,15 @@
       <c r="E17" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="129" t="s">
+      <c r="F17" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="130"/>
-      <c r="H17" s="129" t="s">
+      <c r="G17" s="135"/>
+      <c r="H17" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="131"/>
-      <c r="J17" s="130"/>
+      <c r="I17" s="136"/>
+      <c r="J17" s="135"/>
       <c r="K17" s="55"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -4163,17 +4163,17 @@
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>45000</v>
       </c>
-      <c r="F18" s="123">
+      <c r="F18" s="128">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>139654</v>
       </c>
-      <c r="G18" s="124"/>
-      <c r="H18" s="123">
+      <c r="G18" s="129"/>
+      <c r="H18" s="128">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>140483</v>
       </c>
-      <c r="I18" s="125"/>
-      <c r="J18" s="124"/>
+      <c r="I18" s="130"/>
+      <c r="J18" s="129"/>
       <c r="K18" s="47"/>
     </row>
     <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -4185,31 +4185,20 @@
       <c r="E19" s="61">
         <v>94654</v>
       </c>
-      <c r="F19" s="126">
+      <c r="F19" s="131">
         <v>829</v>
       </c>
-      <c r="G19" s="128"/>
-      <c r="H19" s="126">
+      <c r="G19" s="133"/>
+      <c r="H19" s="131">
         <v>408667</v>
       </c>
-      <c r="I19" s="127"/>
-      <c r="J19" s="128"/>
+      <c r="I19" s="132"/>
+      <c r="J19" s="133"/>
       <c r="K19" s="62"/>
     </row>
     <row r="20" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="F18:G18"/>
@@ -4218,6 +4207,17 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="F19:G19"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="C5:K5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4274,18 +4274,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="124" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
       <c r="L1" s="67"/>
       <c r="M1" s="67"/>
       <c r="N1" s="67"/>
@@ -4314,57 +4314,57 @@
     <row r="4" spans="2:39" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:39" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="106"/>
-      <c r="Y5" s="106"/>
-      <c r="Z5" s="106"/>
-      <c r="AA5" s="106"/>
-      <c r="AB5" s="106"/>
-      <c r="AC5" s="106"/>
-      <c r="AD5" s="106"/>
-      <c r="AE5" s="106"/>
-      <c r="AF5" s="106"/>
-      <c r="AG5" s="106"/>
-      <c r="AH5" s="106"/>
-      <c r="AI5" s="106"/>
-      <c r="AJ5" s="106"/>
-      <c r="AK5" s="106"/>
-      <c r="AL5" s="106"/>
-      <c r="AM5" s="107"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="112"/>
+      <c r="O5" s="112"/>
+      <c r="P5" s="112"/>
+      <c r="Q5" s="112"/>
+      <c r="R5" s="112"/>
+      <c r="S5" s="112"/>
+      <c r="T5" s="112"/>
+      <c r="U5" s="112"/>
+      <c r="V5" s="112"/>
+      <c r="W5" s="112"/>
+      <c r="X5" s="112"/>
+      <c r="Y5" s="112"/>
+      <c r="Z5" s="112"/>
+      <c r="AA5" s="112"/>
+      <c r="AB5" s="112"/>
+      <c r="AC5" s="112"/>
+      <c r="AD5" s="112"/>
+      <c r="AE5" s="112"/>
+      <c r="AF5" s="112"/>
+      <c r="AG5" s="112"/>
+      <c r="AH5" s="112"/>
+      <c r="AI5" s="112"/>
+      <c r="AJ5" s="112"/>
+      <c r="AK5" s="112"/>
+      <c r="AL5" s="112"/>
+      <c r="AM5" s="113"/>
     </row>
     <row r="6" spans="2:39" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
       <c r="H6" s="32"/>
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
@@ -4405,75 +4405,75 @@
         <v>3</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="93" t="s">
+      <c r="D7" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="94"/>
-      <c r="F7" s="93" t="s">
+      <c r="E7" s="93"/>
+      <c r="F7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="94"/>
-      <c r="H7" s="93" t="s">
+      <c r="G7" s="93"/>
+      <c r="H7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="94"/>
-      <c r="J7" s="93" t="s">
+      <c r="I7" s="93"/>
+      <c r="J7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="93" t="s">
+      <c r="K7" s="93"/>
+      <c r="L7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="94"/>
-      <c r="N7" s="93" t="s">
+      <c r="M7" s="93"/>
+      <c r="N7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="94"/>
-      <c r="P7" s="93" t="s">
+      <c r="O7" s="93"/>
+      <c r="P7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="93" t="s">
+      <c r="Q7" s="93"/>
+      <c r="R7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="94"/>
-      <c r="T7" s="93" t="s">
+      <c r="S7" s="93"/>
+      <c r="T7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="U7" s="94"/>
-      <c r="V7" s="93" t="s">
+      <c r="U7" s="93"/>
+      <c r="V7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="W7" s="94"/>
-      <c r="X7" s="93" t="s">
+      <c r="W7" s="93"/>
+      <c r="X7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="Y7" s="94"/>
-      <c r="Z7" s="93" t="s">
+      <c r="Y7" s="93"/>
+      <c r="Z7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AA7" s="94"/>
-      <c r="AB7" s="93" t="s">
+      <c r="AA7" s="93"/>
+      <c r="AB7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="94"/>
-      <c r="AD7" s="93" t="s">
+      <c r="AC7" s="93"/>
+      <c r="AD7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AE7" s="94"/>
-      <c r="AF7" s="93" t="s">
+      <c r="AE7" s="93"/>
+      <c r="AF7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AG7" s="94"/>
-      <c r="AH7" s="93" t="s">
+      <c r="AG7" s="93"/>
+      <c r="AH7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AI7" s="94"/>
-      <c r="AJ7" s="93" t="s">
+      <c r="AI7" s="93"/>
+      <c r="AJ7" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="AK7" s="108"/>
-      <c r="AL7" s="94"/>
+      <c r="AK7" s="92"/>
+      <c r="AL7" s="93"/>
       <c r="AM7" s="2"/>
     </row>
     <row r="8" spans="2:39" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -4481,74 +4481,74 @@
         <v>2</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="95" t="s">
+      <c r="D8" s="94" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="96"/>
-      <c r="F8" s="95" t="s">
+      <c r="F8" s="94" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="96"/>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="94" t="s">
         <v>62</v>
       </c>
       <c r="I8" s="96"/>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="94" t="s">
         <v>63</v>
       </c>
       <c r="K8" s="96"/>
-      <c r="L8" s="95" t="s">
+      <c r="L8" s="94" t="s">
         <v>64</v>
       </c>
       <c r="M8" s="96"/>
-      <c r="N8" s="95" t="s">
+      <c r="N8" s="94" t="s">
         <v>65</v>
       </c>
       <c r="O8" s="96"/>
-      <c r="P8" s="95" t="s">
+      <c r="P8" s="94" t="s">
         <v>66</v>
       </c>
       <c r="Q8" s="96"/>
-      <c r="R8" s="95" t="s">
+      <c r="R8" s="94" t="s">
         <v>67</v>
       </c>
       <c r="S8" s="96"/>
-      <c r="T8" s="95" t="s">
+      <c r="T8" s="94" t="s">
         <v>68</v>
       </c>
       <c r="U8" s="96"/>
-      <c r="V8" s="95" t="s">
+      <c r="V8" s="94" t="s">
         <v>69</v>
       </c>
       <c r="W8" s="96"/>
-      <c r="X8" s="95" t="s">
+      <c r="X8" s="94" t="s">
         <v>70</v>
       </c>
       <c r="Y8" s="96"/>
-      <c r="Z8" s="95" t="s">
+      <c r="Z8" s="94" t="s">
         <v>71</v>
       </c>
       <c r="AA8" s="96"/>
-      <c r="AB8" s="95" t="s">
+      <c r="AB8" s="94" t="s">
         <v>72</v>
       </c>
       <c r="AC8" s="96"/>
-      <c r="AD8" s="95" t="s">
+      <c r="AD8" s="94" t="s">
         <v>73</v>
       </c>
       <c r="AE8" s="96"/>
-      <c r="AF8" s="95" t="s">
+      <c r="AF8" s="94" t="s">
         <v>74</v>
       </c>
       <c r="AG8" s="96"/>
-      <c r="AH8" s="95" t="s">
+      <c r="AH8" s="94" t="s">
         <v>75</v>
       </c>
       <c r="AI8" s="96"/>
-      <c r="AJ8" s="95" t="s">
+      <c r="AJ8" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="AK8" s="98"/>
+      <c r="AK8" s="95"/>
       <c r="AL8" s="96"/>
       <c r="AM8" s="2"/>
     </row>
@@ -4653,10 +4653,10 @@
       <c r="AI9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AJ9" s="100" t="s">
+      <c r="AJ9" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="AK9" s="101"/>
+      <c r="AK9" s="110"/>
       <c r="AL9" s="20" t="s">
         <v>5</v>
       </c>
@@ -5169,66 +5169,66 @@
         <v>28</v>
       </c>
       <c r="F14" s="43"/>
-      <c r="G14" s="134" t="s">
+      <c r="G14" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="135"/>
-      <c r="I14" s="134" t="s">
+      <c r="H14" s="141"/>
+      <c r="I14" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="135"/>
-      <c r="K14" s="134" t="s">
+      <c r="J14" s="141"/>
+      <c r="K14" s="140" t="s">
         <v>92</v>
       </c>
-      <c r="L14" s="135"/>
-      <c r="M14" s="134" t="s">
+      <c r="L14" s="141"/>
+      <c r="M14" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="N14" s="135"/>
-      <c r="O14" s="134" t="s">
+      <c r="N14" s="141"/>
+      <c r="O14" s="140" t="s">
         <v>94</v>
       </c>
-      <c r="P14" s="135"/>
-      <c r="Q14" s="134" t="s">
+      <c r="P14" s="141"/>
+      <c r="Q14" s="140" t="s">
         <v>95</v>
       </c>
-      <c r="R14" s="135"/>
-      <c r="S14" s="134" t="s">
+      <c r="R14" s="141"/>
+      <c r="S14" s="140" t="s">
         <v>96</v>
       </c>
-      <c r="T14" s="140"/>
-      <c r="U14" s="134" t="s">
+      <c r="T14" s="147"/>
+      <c r="U14" s="140" t="s">
         <v>97</v>
       </c>
-      <c r="V14" s="135"/>
-      <c r="W14" s="134" t="s">
+      <c r="V14" s="141"/>
+      <c r="W14" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="X14" s="140"/>
-      <c r="Y14" s="134" t="s">
+      <c r="X14" s="147"/>
+      <c r="Y14" s="140" t="s">
         <v>99</v>
       </c>
-      <c r="Z14" s="135"/>
-      <c r="AA14" s="134" t="s">
+      <c r="Z14" s="141"/>
+      <c r="AA14" s="140" t="s">
         <v>100</v>
       </c>
-      <c r="AB14" s="140"/>
-      <c r="AC14" s="134" t="s">
+      <c r="AB14" s="147"/>
+      <c r="AC14" s="140" t="s">
         <v>101</v>
       </c>
-      <c r="AD14" s="135"/>
-      <c r="AE14" s="140" t="s">
+      <c r="AD14" s="141"/>
+      <c r="AE14" s="147" t="s">
         <v>102</v>
       </c>
-      <c r="AF14" s="140"/>
-      <c r="AG14" s="134" t="s">
+      <c r="AF14" s="147"/>
+      <c r="AG14" s="140" t="s">
         <v>103</v>
       </c>
-      <c r="AH14" s="135"/>
-      <c r="AI14" s="134" t="s">
+      <c r="AH14" s="141"/>
+      <c r="AI14" s="140" t="s">
         <v>104</v>
       </c>
-      <c r="AJ14" s="135"/>
+      <c r="AJ14" s="141"/>
       <c r="AK14" s="43"/>
       <c r="AL14" s="68" t="s">
         <v>105</v>
@@ -5246,81 +5246,81 @@
         <v>45000</v>
       </c>
       <c r="F15" s="66"/>
-      <c r="G15" s="136">
+      <c r="G15" s="142">
         <f t="shared" ref="G15:AL15" ca="1" si="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-2,0)</f>
         <v>355752</v>
       </c>
-      <c r="H15" s="137"/>
-      <c r="I15" s="136">
+      <c r="H15" s="143"/>
+      <c r="I15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>363830</v>
       </c>
-      <c r="J15" s="137"/>
-      <c r="K15" s="136">
+      <c r="J15" s="143"/>
+      <c r="K15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>377274</v>
       </c>
-      <c r="L15" s="137"/>
-      <c r="M15" s="136">
+      <c r="L15" s="143"/>
+      <c r="M15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>380125</v>
       </c>
-      <c r="N15" s="137"/>
-      <c r="O15" s="136">
+      <c r="N15" s="143"/>
+      <c r="O15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>386214</v>
       </c>
-      <c r="P15" s="137"/>
-      <c r="Q15" s="136">
+      <c r="P15" s="143"/>
+      <c r="Q15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>393566</v>
       </c>
-      <c r="R15" s="137"/>
-      <c r="S15" s="136">
+      <c r="R15" s="143"/>
+      <c r="S15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>395638</v>
       </c>
-      <c r="T15" s="141"/>
-      <c r="U15" s="136">
+      <c r="T15" s="148"/>
+      <c r="U15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>399475</v>
       </c>
-      <c r="V15" s="137"/>
-      <c r="W15" s="136">
+      <c r="V15" s="143"/>
+      <c r="W15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>408746</v>
       </c>
-      <c r="X15" s="141"/>
-      <c r="Y15" s="136">
+      <c r="X15" s="148"/>
+      <c r="Y15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>433284</v>
       </c>
-      <c r="Z15" s="137"/>
-      <c r="AA15" s="136">
+      <c r="Z15" s="143"/>
+      <c r="AA15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>458308</v>
       </c>
-      <c r="AB15" s="141"/>
-      <c r="AC15" s="136">
+      <c r="AB15" s="148"/>
+      <c r="AC15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>465907</v>
       </c>
-      <c r="AD15" s="137"/>
-      <c r="AE15" s="141">
+      <c r="AD15" s="143"/>
+      <c r="AE15" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>493817</v>
       </c>
-      <c r="AF15" s="141"/>
-      <c r="AG15" s="136">
+      <c r="AF15" s="148"/>
+      <c r="AG15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>503254</v>
       </c>
-      <c r="AH15" s="137"/>
-      <c r="AI15" s="136">
+      <c r="AH15" s="143"/>
+      <c r="AI15" s="142">
         <f t="shared" ca="1" si="1"/>
         <v>505445</v>
       </c>
-      <c r="AJ15" s="137"/>
+      <c r="AJ15" s="143"/>
       <c r="AK15" s="66"/>
       <c r="AL15" s="69">
         <f t="shared" ca="1" si="1"/>
@@ -5338,66 +5338,66 @@
         <v>310602</v>
       </c>
       <c r="F16" s="49"/>
-      <c r="G16" s="138">
+      <c r="G16" s="144">
         <v>8078</v>
       </c>
-      <c r="H16" s="139"/>
-      <c r="I16" s="138">
+      <c r="H16" s="145"/>
+      <c r="I16" s="144">
         <v>13444</v>
       </c>
-      <c r="J16" s="139"/>
-      <c r="K16" s="138">
+      <c r="J16" s="145"/>
+      <c r="K16" s="144">
         <v>2851</v>
       </c>
-      <c r="L16" s="139"/>
-      <c r="M16" s="138">
+      <c r="L16" s="145"/>
+      <c r="M16" s="144">
         <v>6089</v>
       </c>
-      <c r="N16" s="139"/>
-      <c r="O16" s="138">
+      <c r="N16" s="145"/>
+      <c r="O16" s="144">
         <v>7352</v>
       </c>
-      <c r="P16" s="139"/>
-      <c r="Q16" s="138">
+      <c r="P16" s="145"/>
+      <c r="Q16" s="144">
         <v>2072</v>
       </c>
-      <c r="R16" s="139"/>
-      <c r="S16" s="138">
+      <c r="R16" s="145"/>
+      <c r="S16" s="144">
         <v>3837</v>
       </c>
-      <c r="T16" s="142"/>
-      <c r="U16" s="138">
+      <c r="T16" s="149"/>
+      <c r="U16" s="144">
         <v>9271</v>
       </c>
-      <c r="V16" s="139"/>
-      <c r="W16" s="138">
+      <c r="V16" s="145"/>
+      <c r="W16" s="144">
         <v>24538</v>
       </c>
-      <c r="X16" s="142"/>
-      <c r="Y16" s="138">
+      <c r="X16" s="149"/>
+      <c r="Y16" s="144">
         <v>25024</v>
       </c>
-      <c r="Z16" s="139"/>
-      <c r="AA16" s="138">
+      <c r="Z16" s="145"/>
+      <c r="AA16" s="144">
         <v>7599</v>
       </c>
-      <c r="AB16" s="142"/>
-      <c r="AC16" s="138">
+      <c r="AB16" s="149"/>
+      <c r="AC16" s="144">
         <v>27910</v>
       </c>
-      <c r="AD16" s="139"/>
-      <c r="AE16" s="142">
+      <c r="AD16" s="145"/>
+      <c r="AE16" s="149">
         <v>9437</v>
       </c>
-      <c r="AF16" s="142"/>
-      <c r="AG16" s="138">
+      <c r="AF16" s="149"/>
+      <c r="AG16" s="144">
         <v>2191</v>
       </c>
-      <c r="AH16" s="139"/>
-      <c r="AI16" s="138">
+      <c r="AH16" s="145"/>
+      <c r="AI16" s="144">
         <v>449</v>
       </c>
-      <c r="AJ16" s="139"/>
+      <c r="AJ16" s="145"/>
       <c r="AK16" s="49"/>
       <c r="AL16" s="70">
         <v>43106</v>
@@ -5413,71 +5413,71 @@
       <c r="E17" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="146" t="s">
+      <c r="F17" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="146"/>
-      <c r="H17" s="146" t="s">
+      <c r="G17" s="137"/>
+      <c r="H17" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="146"/>
-      <c r="J17" s="146" t="s">
+      <c r="I17" s="137"/>
+      <c r="J17" s="137" t="s">
         <v>79</v>
       </c>
-      <c r="K17" s="146"/>
-      <c r="L17" s="146" t="s">
+      <c r="K17" s="137"/>
+      <c r="L17" s="137" t="s">
         <v>80</v>
       </c>
-      <c r="M17" s="146"/>
-      <c r="N17" s="146" t="s">
+      <c r="M17" s="137"/>
+      <c r="N17" s="137" t="s">
         <v>81</v>
       </c>
-      <c r="O17" s="146"/>
-      <c r="P17" s="146" t="s">
+      <c r="O17" s="137"/>
+      <c r="P17" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="Q17" s="146"/>
-      <c r="R17" s="146" t="s">
+      <c r="Q17" s="137"/>
+      <c r="R17" s="137" t="s">
         <v>83</v>
       </c>
-      <c r="S17" s="146"/>
-      <c r="T17" s="146" t="s">
+      <c r="S17" s="137"/>
+      <c r="T17" s="137" t="s">
         <v>84</v>
       </c>
-      <c r="U17" s="146"/>
-      <c r="V17" s="146" t="s">
+      <c r="U17" s="137"/>
+      <c r="V17" s="137" t="s">
         <v>85</v>
       </c>
-      <c r="W17" s="146"/>
-      <c r="X17" s="146" t="s">
+      <c r="W17" s="137"/>
+      <c r="X17" s="137" t="s">
         <v>86</v>
       </c>
-      <c r="Y17" s="146"/>
-      <c r="Z17" s="146" t="s">
+      <c r="Y17" s="137"/>
+      <c r="Z17" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="AA17" s="146"/>
-      <c r="AB17" s="146" t="s">
+      <c r="AA17" s="137"/>
+      <c r="AB17" s="137" t="s">
         <v>88</v>
       </c>
-      <c r="AC17" s="146"/>
-      <c r="AD17" s="146" t="s">
+      <c r="AC17" s="137"/>
+      <c r="AD17" s="137" t="s">
         <v>89</v>
       </c>
-      <c r="AE17" s="146"/>
-      <c r="AF17" s="146" t="s">
+      <c r="AE17" s="137"/>
+      <c r="AF17" s="137" t="s">
         <v>90</v>
       </c>
-      <c r="AG17" s="146"/>
-      <c r="AH17" s="146" t="s">
+      <c r="AG17" s="137"/>
+      <c r="AH17" s="137" t="s">
         <v>91</v>
       </c>
-      <c r="AI17" s="146"/>
-      <c r="AJ17" s="146" t="s">
+      <c r="AI17" s="137"/>
+      <c r="AJ17" s="137" t="s">
         <v>77</v>
       </c>
-      <c r="AK17" s="146"/>
-      <c r="AL17" s="146"/>
+      <c r="AK17" s="137"/>
+      <c r="AL17" s="137"/>
       <c r="AM17" s="55"/>
     </row>
     <row r="18" spans="2:39" x14ac:dyDescent="0.2">
@@ -5490,87 +5490,87 @@
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>45000</v>
       </c>
-      <c r="F18" s="147">
+      <c r="F18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>355602</v>
       </c>
-      <c r="G18" s="147"/>
-      <c r="H18" s="147">
+      <c r="G18" s="138"/>
+      <c r="H18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>363680</v>
       </c>
-      <c r="I18" s="147"/>
-      <c r="J18" s="147">
+      <c r="I18" s="138"/>
+      <c r="J18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>377124</v>
       </c>
-      <c r="K18" s="147"/>
-      <c r="L18" s="147">
+      <c r="K18" s="138"/>
+      <c r="L18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>379975</v>
       </c>
-      <c r="M18" s="147"/>
-      <c r="N18" s="147">
+      <c r="M18" s="138"/>
+      <c r="N18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>386064</v>
       </c>
-      <c r="O18" s="147"/>
-      <c r="P18" s="147">
+      <c r="O18" s="138"/>
+      <c r="P18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>393416</v>
       </c>
-      <c r="Q18" s="147"/>
-      <c r="R18" s="147">
+      <c r="Q18" s="138"/>
+      <c r="R18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>395488</v>
       </c>
-      <c r="S18" s="147"/>
-      <c r="T18" s="147">
+      <c r="S18" s="138"/>
+      <c r="T18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>399325</v>
       </c>
-      <c r="U18" s="147"/>
-      <c r="V18" s="147">
+      <c r="U18" s="138"/>
+      <c r="V18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>408596</v>
       </c>
-      <c r="W18" s="147"/>
-      <c r="X18" s="147">
+      <c r="W18" s="138"/>
+      <c r="X18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>433134</v>
       </c>
-      <c r="Y18" s="147"/>
-      <c r="Z18" s="147">
+      <c r="Y18" s="138"/>
+      <c r="Z18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>458158</v>
       </c>
-      <c r="AA18" s="147"/>
-      <c r="AB18" s="147">
+      <c r="AA18" s="138"/>
+      <c r="AB18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>465757</v>
       </c>
-      <c r="AC18" s="147"/>
-      <c r="AD18" s="147">
+      <c r="AC18" s="138"/>
+      <c r="AD18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>493667</v>
       </c>
-      <c r="AE18" s="147"/>
-      <c r="AF18" s="147">
+      <c r="AE18" s="138"/>
+      <c r="AF18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>503104</v>
       </c>
-      <c r="AG18" s="147"/>
-      <c r="AH18" s="147">
+      <c r="AG18" s="138"/>
+      <c r="AH18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>505295</v>
       </c>
-      <c r="AI18" s="147"/>
-      <c r="AJ18" s="147">
+      <c r="AI18" s="138"/>
+      <c r="AJ18" s="138">
         <f ca="1">OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),-5,0)</f>
         <v>505819</v>
       </c>
-      <c r="AK18" s="147"/>
-      <c r="AL18" s="147"/>
+      <c r="AK18" s="138"/>
+      <c r="AL18" s="138"/>
       <c r="AM18" s="47"/>
     </row>
     <row r="19" spans="2:39" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -5582,201 +5582,152 @@
       <c r="E19" s="73">
         <v>310602</v>
       </c>
-      <c r="F19" s="145">
+      <c r="F19" s="139">
         <v>8078</v>
       </c>
-      <c r="G19" s="145"/>
-      <c r="H19" s="145">
+      <c r="G19" s="139"/>
+      <c r="H19" s="139">
         <v>13444</v>
       </c>
-      <c r="I19" s="145"/>
-      <c r="J19" s="145">
+      <c r="I19" s="139"/>
+      <c r="J19" s="139">
         <v>2851</v>
       </c>
-      <c r="K19" s="145"/>
-      <c r="L19" s="145">
+      <c r="K19" s="139"/>
+      <c r="L19" s="139">
         <v>6089</v>
       </c>
-      <c r="M19" s="145"/>
-      <c r="N19" s="145">
+      <c r="M19" s="139"/>
+      <c r="N19" s="139">
         <v>7352</v>
       </c>
-      <c r="O19" s="145"/>
-      <c r="P19" s="145">
+      <c r="O19" s="139"/>
+      <c r="P19" s="139">
         <v>2072</v>
       </c>
-      <c r="Q19" s="145"/>
-      <c r="R19" s="145">
+      <c r="Q19" s="139"/>
+      <c r="R19" s="139">
         <v>3837</v>
       </c>
-      <c r="S19" s="145"/>
-      <c r="T19" s="145">
+      <c r="S19" s="139"/>
+      <c r="T19" s="139">
         <v>9271</v>
       </c>
-      <c r="U19" s="145"/>
-      <c r="V19" s="145">
+      <c r="U19" s="139"/>
+      <c r="V19" s="139">
         <v>24538</v>
       </c>
-      <c r="W19" s="145"/>
-      <c r="X19" s="145">
+      <c r="W19" s="139"/>
+      <c r="X19" s="139">
         <v>25024</v>
       </c>
-      <c r="Y19" s="145"/>
-      <c r="Z19" s="145">
+      <c r="Y19" s="139"/>
+      <c r="Z19" s="139">
         <v>7599</v>
       </c>
-      <c r="AA19" s="145"/>
-      <c r="AB19" s="145">
+      <c r="AA19" s="139"/>
+      <c r="AB19" s="139">
         <v>27910</v>
       </c>
-      <c r="AC19" s="145"/>
-      <c r="AD19" s="145">
+      <c r="AC19" s="139"/>
+      <c r="AD19" s="139">
         <v>9437</v>
       </c>
-      <c r="AE19" s="145"/>
-      <c r="AF19" s="145">
+      <c r="AE19" s="139"/>
+      <c r="AF19" s="139">
         <v>2191</v>
       </c>
-      <c r="AG19" s="145"/>
-      <c r="AH19" s="145">
+      <c r="AG19" s="139"/>
+      <c r="AH19" s="139">
         <v>524</v>
       </c>
-      <c r="AI19" s="145"/>
-      <c r="AJ19" s="145">
+      <c r="AI19" s="139"/>
+      <c r="AJ19" s="139">
         <v>43331</v>
       </c>
-      <c r="AK19" s="145"/>
-      <c r="AL19" s="145"/>
+      <c r="AK19" s="139"/>
+      <c r="AL19" s="139"/>
       <c r="AM19" s="62"/>
     </row>
     <row r="20" spans="2:39" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B22" s="144" t="s">
+      <c r="B22" s="146" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="144"/>
-      <c r="D22" s="144"/>
-      <c r="E22" s="144"/>
-      <c r="F22" s="144"/>
-      <c r="G22" s="144"/>
-      <c r="H22" s="144"/>
-      <c r="I22" s="144"/>
-      <c r="J22" s="144"/>
-      <c r="K22" s="144"/>
-      <c r="L22" s="144"/>
-      <c r="M22" s="144"/>
-      <c r="N22" s="144"/>
-      <c r="O22" s="144"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="146"/>
+      <c r="J22" s="146"/>
+      <c r="K22" s="146"/>
+      <c r="L22" s="146"/>
+      <c r="M22" s="146"/>
+      <c r="N22" s="146"/>
+      <c r="O22" s="146"/>
     </row>
     <row r="23" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B23" s="143" t="s">
+      <c r="B23" s="150" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="143"/>
-      <c r="D23" s="143"/>
-      <c r="E23" s="143"/>
-      <c r="F23" s="143"/>
-      <c r="G23" s="143"/>
-      <c r="H23" s="143"/>
-      <c r="I23" s="143"/>
-      <c r="J23" s="143"/>
-      <c r="K23" s="143"/>
-      <c r="L23" s="143"/>
-      <c r="M23" s="143"/>
-      <c r="N23" s="143"/>
-      <c r="O23" s="143"/>
+      <c r="C23" s="150"/>
+      <c r="D23" s="150"/>
+      <c r="E23" s="150"/>
+      <c r="F23" s="150"/>
+      <c r="G23" s="150"/>
+      <c r="H23" s="150"/>
+      <c r="I23" s="150"/>
+      <c r="J23" s="150"/>
+      <c r="K23" s="150"/>
+      <c r="L23" s="150"/>
+      <c r="M23" s="150"/>
+      <c r="N23" s="150"/>
+      <c r="O23" s="150"/>
     </row>
     <row r="25" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B25" s="143" t="s">
+      <c r="B25" s="150" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="143"/>
-      <c r="D25" s="143"/>
-      <c r="E25" s="143"/>
-      <c r="F25" s="143"/>
-      <c r="G25" s="143"/>
-      <c r="H25" s="143"/>
-      <c r="I25" s="143"/>
-      <c r="J25" s="143"/>
-      <c r="K25" s="143"/>
-      <c r="L25" s="143"/>
-      <c r="M25" s="143"/>
-      <c r="N25" s="143"/>
-      <c r="O25" s="143"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="150"/>
+      <c r="G25" s="150"/>
+      <c r="H25" s="150"/>
+      <c r="I25" s="150"/>
+      <c r="J25" s="150"/>
+      <c r="K25" s="150"/>
+      <c r="L25" s="150"/>
+      <c r="M25" s="150"/>
+      <c r="N25" s="150"/>
+      <c r="O25" s="150"/>
     </row>
   </sheetData>
   <mergeCells count="134">
-    <mergeCell ref="C5:AM5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="AJ7:AL7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="AJ17:AL17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="AJ18:AL18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="AJ19:AL19"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="AJ8:AL8"/>
-    <mergeCell ref="AJ9:AK9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="AH18:AI18"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="AD8:AE8"/>
-    <mergeCell ref="AF8:AG8"/>
-    <mergeCell ref="AH8:AI8"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AD17:AE17"/>
-    <mergeCell ref="AI14:AJ14"/>
-    <mergeCell ref="AI15:AJ15"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AG16:AH16"/>
+    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AE16:AF16"/>
+    <mergeCell ref="B23:O23"/>
+    <mergeCell ref="B25:O25"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="AI16:AJ16"/>
     <mergeCell ref="B22:O22"/>
@@ -5801,24 +5752,18 @@
     <mergeCell ref="AF18:AG18"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="B23:O23"/>
-    <mergeCell ref="B25:O25"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="AH18:AI18"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="AH8:AI8"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AD17:AE17"/>
+    <mergeCell ref="AI14:AJ14"/>
+    <mergeCell ref="AI15:AJ15"/>
     <mergeCell ref="Y14:Z14"/>
     <mergeCell ref="Y15:Z15"/>
     <mergeCell ref="Y16:Z16"/>
@@ -5831,15 +5776,70 @@
     <mergeCell ref="W14:X14"/>
     <mergeCell ref="W15:X15"/>
     <mergeCell ref="W16:X16"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AG16:AH16"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AE16:AF16"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="AJ17:AL17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="AJ18:AL18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="AJ19:AL19"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="AJ8:AL8"/>
+    <mergeCell ref="AJ9:AK9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="C5:AM5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="AJ7:AL7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AH7:AI7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>